<commit_message>
Updated missing country data
</commit_message>
<xml_diff>
--- a/tabular/missing_data/countries_locations.xlsx
+++ b/tabular/missing_data/countries_locations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26500" yWindow="3360" windowWidth="15080" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="26360" yWindow="3380" windowWidth="15080" windowHeight="16760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2122" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2852" uniqueCount="1272">
   <si>
     <t>KY620313</t>
   </si>
@@ -2738,6 +2738,1104 @@
   </si>
   <si>
     <t>GBR</t>
+  </si>
+  <si>
+    <t>AB061927</t>
+  </si>
+  <si>
+    <t>AB061928</t>
+  </si>
+  <si>
+    <t>AB061929</t>
+  </si>
+  <si>
+    <t>AB061930</t>
+  </si>
+  <si>
+    <t>AB061931</t>
+  </si>
+  <si>
+    <t>AB061932</t>
+  </si>
+  <si>
+    <t>AB061933</t>
+  </si>
+  <si>
+    <t>AB061934</t>
+  </si>
+  <si>
+    <t>AB061935</t>
+  </si>
+  <si>
+    <t>AB061936</t>
+  </si>
+  <si>
+    <t>AB061937</t>
+  </si>
+  <si>
+    <t>AB061938</t>
+  </si>
+  <si>
+    <t>AB061939</t>
+  </si>
+  <si>
+    <t>AB061940</t>
+  </si>
+  <si>
+    <t>AB061941</t>
+  </si>
+  <si>
+    <t>AB061942</t>
+  </si>
+  <si>
+    <t>AB061943</t>
+  </si>
+  <si>
+    <t>AB061944</t>
+  </si>
+  <si>
+    <t>AB061945</t>
+  </si>
+  <si>
+    <t>AB061946</t>
+  </si>
+  <si>
+    <t>AB061947</t>
+  </si>
+  <si>
+    <t>AB061948</t>
+  </si>
+  <si>
+    <t>AB061949</t>
+  </si>
+  <si>
+    <t>AB061950</t>
+  </si>
+  <si>
+    <t>AB061951</t>
+  </si>
+  <si>
+    <t>AB061952</t>
+  </si>
+  <si>
+    <t>AB061953</t>
+  </si>
+  <si>
+    <t>AB061954</t>
+  </si>
+  <si>
+    <t>AB061955</t>
+  </si>
+  <si>
+    <t>AB061956</t>
+  </si>
+  <si>
+    <t>AB061957</t>
+  </si>
+  <si>
+    <t>AB061958</t>
+  </si>
+  <si>
+    <t>AB061959</t>
+  </si>
+  <si>
+    <t>AB061960</t>
+  </si>
+  <si>
+    <t>AB061961</t>
+  </si>
+  <si>
+    <t>AB061962</t>
+  </si>
+  <si>
+    <t>AB061963</t>
+  </si>
+  <si>
+    <t>AB061964</t>
+  </si>
+  <si>
+    <t>AB061965</t>
+  </si>
+  <si>
+    <t>AB061966</t>
+  </si>
+  <si>
+    <t>AB061967</t>
+  </si>
+  <si>
+    <t>AB061968</t>
+  </si>
+  <si>
+    <t>AB061969</t>
+  </si>
+  <si>
+    <t>AB061970</t>
+  </si>
+  <si>
+    <t>AB061971</t>
+  </si>
+  <si>
+    <t>AB061972</t>
+  </si>
+  <si>
+    <t>AB061973</t>
+  </si>
+  <si>
+    <t>AB061974</t>
+  </si>
+  <si>
+    <t>AB061975</t>
+  </si>
+  <si>
+    <t>AB061976</t>
+  </si>
+  <si>
+    <t>AB061977</t>
+  </si>
+  <si>
+    <t>AB061978</t>
+  </si>
+  <si>
+    <t>AB061979</t>
+  </si>
+  <si>
+    <t>AB061980</t>
+  </si>
+  <si>
+    <t>AB061981</t>
+  </si>
+  <si>
+    <t>AB061982</t>
+  </si>
+  <si>
+    <t>AB061983</t>
+  </si>
+  <si>
+    <t>AB061984</t>
+  </si>
+  <si>
+    <t>AB061985</t>
+  </si>
+  <si>
+    <t>AB061986</t>
+  </si>
+  <si>
+    <t>AB061987</t>
+  </si>
+  <si>
+    <t>AB061988</t>
+  </si>
+  <si>
+    <t>AB061989</t>
+  </si>
+  <si>
+    <t>AB061990</t>
+  </si>
+  <si>
+    <t>AB061991</t>
+  </si>
+  <si>
+    <t>AB061992</t>
+  </si>
+  <si>
+    <t>AB061993</t>
+  </si>
+  <si>
+    <t>AB061994</t>
+  </si>
+  <si>
+    <t>AB061995</t>
+  </si>
+  <si>
+    <t>AB061996</t>
+  </si>
+  <si>
+    <t>AB061997</t>
+  </si>
+  <si>
+    <t>AB061998</t>
+  </si>
+  <si>
+    <t>AB061999</t>
+  </si>
+  <si>
+    <t>AB062000</t>
+  </si>
+  <si>
+    <t>AB062001</t>
+  </si>
+  <si>
+    <t>AB062002</t>
+  </si>
+  <si>
+    <t>AB062003</t>
+  </si>
+  <si>
+    <t>AB062004</t>
+  </si>
+  <si>
+    <t>AB062005</t>
+  </si>
+  <si>
+    <t>AB062006</t>
+  </si>
+  <si>
+    <t>AB062007</t>
+  </si>
+  <si>
+    <t>AB062008</t>
+  </si>
+  <si>
+    <t>AB062009</t>
+  </si>
+  <si>
+    <t>AB062010</t>
+  </si>
+  <si>
+    <t>AB062011</t>
+  </si>
+  <si>
+    <t>AB062012</t>
+  </si>
+  <si>
+    <t>AB062013</t>
+  </si>
+  <si>
+    <t>AB062014</t>
+  </si>
+  <si>
+    <t>AB062015</t>
+  </si>
+  <si>
+    <t>AB062016</t>
+  </si>
+  <si>
+    <t>AB062017</t>
+  </si>
+  <si>
+    <t>AB062018</t>
+  </si>
+  <si>
+    <t>AB062019</t>
+  </si>
+  <si>
+    <t>AB062020</t>
+  </si>
+  <si>
+    <t>AB062021</t>
+  </si>
+  <si>
+    <t>AB062022</t>
+  </si>
+  <si>
+    <t>AB062023</t>
+  </si>
+  <si>
+    <t>AB062024</t>
+  </si>
+  <si>
+    <t>AB062025</t>
+  </si>
+  <si>
+    <t>AB062026</t>
+  </si>
+  <si>
+    <t>AB062173</t>
+  </si>
+  <si>
+    <t>AB062174</t>
+  </si>
+  <si>
+    <t>AB062175</t>
+  </si>
+  <si>
+    <t>AB062176</t>
+  </si>
+  <si>
+    <t>AB062177</t>
+  </si>
+  <si>
+    <t>AB062178</t>
+  </si>
+  <si>
+    <t>AB062179</t>
+  </si>
+  <si>
+    <t>AB062180</t>
+  </si>
+  <si>
+    <t>AB062181</t>
+  </si>
+  <si>
+    <t>AB062182</t>
+  </si>
+  <si>
+    <t>AB062183</t>
+  </si>
+  <si>
+    <t>AB062184</t>
+  </si>
+  <si>
+    <t>AB062185</t>
+  </si>
+  <si>
+    <t>AB062186</t>
+  </si>
+  <si>
+    <t>AB062187</t>
+  </si>
+  <si>
+    <t>AB062188</t>
+  </si>
+  <si>
+    <t>AB062189</t>
+  </si>
+  <si>
+    <t>AB062190</t>
+  </si>
+  <si>
+    <t>AB062191</t>
+  </si>
+  <si>
+    <t>AB062192</t>
+  </si>
+  <si>
+    <t>AB062193</t>
+  </si>
+  <si>
+    <t>AB062194</t>
+  </si>
+  <si>
+    <t>AB062195</t>
+  </si>
+  <si>
+    <t>AB062196</t>
+  </si>
+  <si>
+    <t>AB062197</t>
+  </si>
+  <si>
+    <t>AB062198</t>
+  </si>
+  <si>
+    <t>AB062199</t>
+  </si>
+  <si>
+    <t>AB062200</t>
+  </si>
+  <si>
+    <t>AB062201</t>
+  </si>
+  <si>
+    <t>AB062202</t>
+  </si>
+  <si>
+    <t>AB062203</t>
+  </si>
+  <si>
+    <t>AB062204</t>
+  </si>
+  <si>
+    <t>AB062205</t>
+  </si>
+  <si>
+    <t>AB062206</t>
+  </si>
+  <si>
+    <t>AB062207</t>
+  </si>
+  <si>
+    <t>AB062208</t>
+  </si>
+  <si>
+    <t>AB062209</t>
+  </si>
+  <si>
+    <t>AB062210</t>
+  </si>
+  <si>
+    <t>AB062211</t>
+  </si>
+  <si>
+    <t>AB062212</t>
+  </si>
+  <si>
+    <t>AB062213</t>
+  </si>
+  <si>
+    <t>AB062214</t>
+  </si>
+  <si>
+    <t>AB062215</t>
+  </si>
+  <si>
+    <t>AB062216</t>
+  </si>
+  <si>
+    <t>AB062217</t>
+  </si>
+  <si>
+    <t>AB062218</t>
+  </si>
+  <si>
+    <t>AB062219</t>
+  </si>
+  <si>
+    <t>AB062220</t>
+  </si>
+  <si>
+    <t>AB062221</t>
+  </si>
+  <si>
+    <t>AB062222</t>
+  </si>
+  <si>
+    <t>AB062223</t>
+  </si>
+  <si>
+    <t>AB062224</t>
+  </si>
+  <si>
+    <t>AB062225</t>
+  </si>
+  <si>
+    <t>AB062226</t>
+  </si>
+  <si>
+    <t>AB062227</t>
+  </si>
+  <si>
+    <t>AB062228</t>
+  </si>
+  <si>
+    <t>AB062229</t>
+  </si>
+  <si>
+    <t>AB062230</t>
+  </si>
+  <si>
+    <t>AB062231</t>
+  </si>
+  <si>
+    <t>AB062232</t>
+  </si>
+  <si>
+    <t>AB062233</t>
+  </si>
+  <si>
+    <t>AB062234</t>
+  </si>
+  <si>
+    <t>AB062235</t>
+  </si>
+  <si>
+    <t>AB062236</t>
+  </si>
+  <si>
+    <t>AB062237</t>
+  </si>
+  <si>
+    <t>AB062238</t>
+  </si>
+  <si>
+    <t>AB062239</t>
+  </si>
+  <si>
+    <t>AB062240</t>
+  </si>
+  <si>
+    <t>AB062241</t>
+  </si>
+  <si>
+    <t>AB062242</t>
+  </si>
+  <si>
+    <t>AB062243</t>
+  </si>
+  <si>
+    <t>AB062244</t>
+  </si>
+  <si>
+    <t>AB062245</t>
+  </si>
+  <si>
+    <t>AB062246</t>
+  </si>
+  <si>
+    <t>AB062247</t>
+  </si>
+  <si>
+    <t>AB062248</t>
+  </si>
+  <si>
+    <t>AB062249</t>
+  </si>
+  <si>
+    <t>AB062250</t>
+  </si>
+  <si>
+    <t>AB062251</t>
+  </si>
+  <si>
+    <t>AB062252</t>
+  </si>
+  <si>
+    <t>AB062253</t>
+  </si>
+  <si>
+    <t>AB062254</t>
+  </si>
+  <si>
+    <t>AB062255</t>
+  </si>
+  <si>
+    <t>AB062256</t>
+  </si>
+  <si>
+    <t>AB062257</t>
+  </si>
+  <si>
+    <t>AB062258</t>
+  </si>
+  <si>
+    <t>AB062259</t>
+  </si>
+  <si>
+    <t>AB062260</t>
+  </si>
+  <si>
+    <t>AB062261</t>
+  </si>
+  <si>
+    <t>AB062262</t>
+  </si>
+  <si>
+    <t>AB062263</t>
+  </si>
+  <si>
+    <t>AB062264</t>
+  </si>
+  <si>
+    <t>AB062265</t>
+  </si>
+  <si>
+    <t>AB062266</t>
+  </si>
+  <si>
+    <t>AB062267</t>
+  </si>
+  <si>
+    <t>AB062268</t>
+  </si>
+  <si>
+    <t>AB062269</t>
+  </si>
+  <si>
+    <t>AB062270</t>
+  </si>
+  <si>
+    <t>AB062271</t>
+  </si>
+  <si>
+    <t>AB062272</t>
+  </si>
+  <si>
+    <t>AB072043</t>
+  </si>
+  <si>
+    <t>AB072044</t>
+  </si>
+  <si>
+    <t>AB072045</t>
+  </si>
+  <si>
+    <t>AB072046</t>
+  </si>
+  <si>
+    <t>AB072047</t>
+  </si>
+  <si>
+    <t>AB072048</t>
+  </si>
+  <si>
+    <t>AB072049</t>
+  </si>
+  <si>
+    <t>AB072050</t>
+  </si>
+  <si>
+    <t>AB072051</t>
+  </si>
+  <si>
+    <t>AB072052</t>
+  </si>
+  <si>
+    <t>AB072053</t>
+  </si>
+  <si>
+    <t>AB072054</t>
+  </si>
+  <si>
+    <t>AB072055</t>
+  </si>
+  <si>
+    <t>AB072056</t>
+  </si>
+  <si>
+    <t>AB072057</t>
+  </si>
+  <si>
+    <t>AB072058</t>
+  </si>
+  <si>
+    <t>AB072059</t>
+  </si>
+  <si>
+    <t>AB072060</t>
+  </si>
+  <si>
+    <t>AB072061</t>
+  </si>
+  <si>
+    <t>AB072062</t>
+  </si>
+  <si>
+    <t>AB072063</t>
+  </si>
+  <si>
+    <t>AB072064</t>
+  </si>
+  <si>
+    <t>AB072065</t>
+  </si>
+  <si>
+    <t>AB072066</t>
+  </si>
+  <si>
+    <t>AB072067</t>
+  </si>
+  <si>
+    <t>AB072068</t>
+  </si>
+  <si>
+    <t>AB072069</t>
+  </si>
+  <si>
+    <t>AB072070</t>
+  </si>
+  <si>
+    <t>AB072071</t>
+  </si>
+  <si>
+    <t>AB072072</t>
+  </si>
+  <si>
+    <t>AB072073</t>
+  </si>
+  <si>
+    <t>AB072074</t>
+  </si>
+  <si>
+    <t>AB072075</t>
+  </si>
+  <si>
+    <t>AB072076</t>
+  </si>
+  <si>
+    <t>AB072077</t>
+  </si>
+  <si>
+    <t>AB072078</t>
+  </si>
+  <si>
+    <t>AB072079</t>
+  </si>
+  <si>
+    <t>AB072080</t>
+  </si>
+  <si>
+    <t>AB072081</t>
+  </si>
+  <si>
+    <t>AB072082</t>
+  </si>
+  <si>
+    <t>AB072083</t>
+  </si>
+  <si>
+    <t>AB072084</t>
+  </si>
+  <si>
+    <t>AB072085</t>
+  </si>
+  <si>
+    <t>AB072086</t>
+  </si>
+  <si>
+    <t>AB072087</t>
+  </si>
+  <si>
+    <t>AB072088</t>
+  </si>
+  <si>
+    <t>AB072089</t>
+  </si>
+  <si>
+    <t>AB072090</t>
+  </si>
+  <si>
+    <t>AB072091</t>
+  </si>
+  <si>
+    <t>AB072092</t>
+  </si>
+  <si>
+    <t>AB072093</t>
+  </si>
+  <si>
+    <t>AB072094</t>
+  </si>
+  <si>
+    <t>AB072095</t>
+  </si>
+  <si>
+    <t>AB072096</t>
+  </si>
+  <si>
+    <t>AB072097</t>
+  </si>
+  <si>
+    <t>AB072098</t>
+  </si>
+  <si>
+    <t>AB072099</t>
+  </si>
+  <si>
+    <t>AB072100</t>
+  </si>
+  <si>
+    <t>AB072101</t>
+  </si>
+  <si>
+    <t>AB072102</t>
+  </si>
+  <si>
+    <t>AB072103</t>
+  </si>
+  <si>
+    <t>AB072104</t>
+  </si>
+  <si>
+    <t>AB072105</t>
+  </si>
+  <si>
+    <t>AB072106</t>
+  </si>
+  <si>
+    <t>AB072107</t>
+  </si>
+  <si>
+    <t>AB072108</t>
+  </si>
+  <si>
+    <t>AB072109</t>
+  </si>
+  <si>
+    <t>AB072110</t>
+  </si>
+  <si>
+    <t>AB072111</t>
+  </si>
+  <si>
+    <t>AB072112</t>
+  </si>
+  <si>
+    <t>AB072113</t>
+  </si>
+  <si>
+    <t>AB077701</t>
+  </si>
+  <si>
+    <t>AB077702</t>
+  </si>
+  <si>
+    <t>AB077703</t>
+  </si>
+  <si>
+    <t>AB077704</t>
+  </si>
+  <si>
+    <t>AB077705</t>
+  </si>
+  <si>
+    <t>AB077706</t>
+  </si>
+  <si>
+    <t>AB077707</t>
+  </si>
+  <si>
+    <t>AB077708</t>
+  </si>
+  <si>
+    <t>AB077709</t>
+  </si>
+  <si>
+    <t>AB077710</t>
+  </si>
+  <si>
+    <t>AB077711</t>
+  </si>
+  <si>
+    <t>AB077712</t>
+  </si>
+  <si>
+    <t>AB077713</t>
+  </si>
+  <si>
+    <t>AB077714</t>
+  </si>
+  <si>
+    <t>AB077715</t>
+  </si>
+  <si>
+    <t>AB077716</t>
+  </si>
+  <si>
+    <t>AB077717</t>
+  </si>
+  <si>
+    <t>AB077718</t>
+  </si>
+  <si>
+    <t>AB077719</t>
+  </si>
+  <si>
+    <t>AB077720</t>
+  </si>
+  <si>
+    <t>AB077721</t>
+  </si>
+  <si>
+    <t>AB077722</t>
+  </si>
+  <si>
+    <t>AB077723</t>
+  </si>
+  <si>
+    <t>AB077724</t>
+  </si>
+  <si>
+    <t>AB077725</t>
+  </si>
+  <si>
+    <t>AB077726</t>
+  </si>
+  <si>
+    <t>AB077727</t>
+  </si>
+  <si>
+    <t>AB077728</t>
+  </si>
+  <si>
+    <t>AB077729</t>
+  </si>
+  <si>
+    <t>AB077730</t>
+  </si>
+  <si>
+    <t>AB077731</t>
+  </si>
+  <si>
+    <t>AB077732</t>
+  </si>
+  <si>
+    <t>AB077733</t>
+  </si>
+  <si>
+    <t>AB077734</t>
+  </si>
+  <si>
+    <t>AB077735</t>
+  </si>
+  <si>
+    <t>AB077736</t>
+  </si>
+  <si>
+    <t>AB077737</t>
+  </si>
+  <si>
+    <t>AB077738</t>
+  </si>
+  <si>
+    <t>AB077739</t>
+  </si>
+  <si>
+    <t>AB077740</t>
+  </si>
+  <si>
+    <t>AB077741</t>
+  </si>
+  <si>
+    <t>AB077742</t>
+  </si>
+  <si>
+    <t>AB077743</t>
+  </si>
+  <si>
+    <t>AB077744</t>
+  </si>
+  <si>
+    <t>AB077745</t>
+  </si>
+  <si>
+    <t>AB077746</t>
+  </si>
+  <si>
+    <t>AB077747</t>
+  </si>
+  <si>
+    <t>AB285035</t>
+  </si>
+  <si>
+    <t>AB285036</t>
+  </si>
+  <si>
+    <t>AB285037</t>
+  </si>
+  <si>
+    <t>AB285038</t>
+  </si>
+  <si>
+    <t>AB285039</t>
+  </si>
+  <si>
+    <t>AB285040</t>
+  </si>
+  <si>
+    <t>AB285041</t>
+  </si>
+  <si>
+    <t>AB285042</t>
+  </si>
+  <si>
+    <t>AB285043</t>
+  </si>
+  <si>
+    <t>AB285044</t>
+  </si>
+  <si>
+    <t>AB285045</t>
+  </si>
+  <si>
+    <t>AB285046</t>
+  </si>
+  <si>
+    <t>AB285047</t>
+  </si>
+  <si>
+    <t>AB285048</t>
+  </si>
+  <si>
+    <t>AB285049</t>
+  </si>
+  <si>
+    <t>AB285050</t>
+  </si>
+  <si>
+    <t>AB285051</t>
+  </si>
+  <si>
+    <t>AB285052</t>
+  </si>
+  <si>
+    <t>AB285053</t>
+  </si>
+  <si>
+    <t>AB285054</t>
+  </si>
+  <si>
+    <t>AB285055</t>
+  </si>
+  <si>
+    <t>AB285056</t>
+  </si>
+  <si>
+    <t>AB285057</t>
+  </si>
+  <si>
+    <t>AB285058</t>
+  </si>
+  <si>
+    <t>AB285059</t>
+  </si>
+  <si>
+    <t>AB285060</t>
+  </si>
+  <si>
+    <t>AB285061</t>
+  </si>
+  <si>
+    <t>AB285062</t>
+  </si>
+  <si>
+    <t>AB285063</t>
+  </si>
+  <si>
+    <t>AB285064</t>
+  </si>
+  <si>
+    <t>AB285065</t>
+  </si>
+  <si>
+    <t>AB285066</t>
+  </si>
+  <si>
+    <t>AB285067</t>
+  </si>
+  <si>
+    <t>AB285068</t>
+  </si>
+  <si>
+    <t>AB285069</t>
+  </si>
+  <si>
+    <t>AB285070</t>
+  </si>
+  <si>
+    <t>AB285071</t>
+  </si>
+  <si>
+    <t>AB285072</t>
+  </si>
+  <si>
+    <t>AB285073</t>
+  </si>
+  <si>
+    <t>AB285074</t>
+  </si>
+  <si>
+    <t>AB285075</t>
+  </si>
+  <si>
+    <t>AB285076</t>
+  </si>
+  <si>
+    <t>AB285077</t>
+  </si>
+  <si>
+    <t>AB285078</t>
+  </si>
+  <si>
+    <t>AB285079</t>
+  </si>
+  <si>
+    <t>AB285080</t>
+  </si>
+  <si>
+    <t>AB285081</t>
+  </si>
+  <si>
+    <t>JPN</t>
   </si>
 </sst>
 </file>
@@ -2781,7 +3879,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2806,6 +3904,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2816,7 +3920,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2846,14 +3950,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2868,6 +3977,8 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2882,6 +3993,8 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3211,10 +4324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D894"/>
+  <dimension ref="A1:D1259"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D894"/>
+    <sheetView tabSelected="1" topLeftCell="A1209" workbookViewId="0">
+      <selection activeCell="B1209" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13951,6 +15064,3656 @@
       <c r="D894" s="2">
         <v>26311892</v>
       </c>
+    </row>
+    <row r="895" spans="1:4">
+      <c r="A895" s="4" t="s">
+        <v>906</v>
+      </c>
+      <c r="B895" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C895" s="4"/>
+      <c r="D895" s="4"/>
+    </row>
+    <row r="896" spans="1:4">
+      <c r="A896" s="4" t="s">
+        <v>907</v>
+      </c>
+      <c r="B896" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C896" s="4"/>
+      <c r="D896" s="4"/>
+    </row>
+    <row r="897" spans="1:4">
+      <c r="A897" s="4" t="s">
+        <v>908</v>
+      </c>
+      <c r="B897" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C897" s="4"/>
+      <c r="D897" s="4"/>
+    </row>
+    <row r="898" spans="1:4">
+      <c r="A898" s="4" t="s">
+        <v>909</v>
+      </c>
+      <c r="B898" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C898" s="4"/>
+      <c r="D898" s="4"/>
+    </row>
+    <row r="899" spans="1:4">
+      <c r="A899" s="4" t="s">
+        <v>910</v>
+      </c>
+      <c r="B899" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C899" s="4"/>
+      <c r="D899" s="4"/>
+    </row>
+    <row r="900" spans="1:4">
+      <c r="A900" s="4" t="s">
+        <v>911</v>
+      </c>
+      <c r="B900" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C900" s="4"/>
+      <c r="D900" s="4"/>
+    </row>
+    <row r="901" spans="1:4">
+      <c r="A901" s="4" t="s">
+        <v>912</v>
+      </c>
+      <c r="B901" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C901" s="4"/>
+      <c r="D901" s="4"/>
+    </row>
+    <row r="902" spans="1:4">
+      <c r="A902" s="4" t="s">
+        <v>913</v>
+      </c>
+      <c r="B902" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C902" s="4"/>
+      <c r="D902" s="4"/>
+    </row>
+    <row r="903" spans="1:4">
+      <c r="A903" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="B903" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C903" s="4"/>
+      <c r="D903" s="4"/>
+    </row>
+    <row r="904" spans="1:4">
+      <c r="A904" s="4" t="s">
+        <v>915</v>
+      </c>
+      <c r="B904" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C904" s="4"/>
+      <c r="D904" s="4"/>
+    </row>
+    <row r="905" spans="1:4">
+      <c r="A905" s="4" t="s">
+        <v>916</v>
+      </c>
+      <c r="B905" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C905" s="4"/>
+      <c r="D905" s="4"/>
+    </row>
+    <row r="906" spans="1:4">
+      <c r="A906" s="4" t="s">
+        <v>917</v>
+      </c>
+      <c r="B906" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C906" s="4"/>
+      <c r="D906" s="4"/>
+    </row>
+    <row r="907" spans="1:4">
+      <c r="A907" s="4" t="s">
+        <v>918</v>
+      </c>
+      <c r="B907" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C907" s="4"/>
+      <c r="D907" s="4"/>
+    </row>
+    <row r="908" spans="1:4">
+      <c r="A908" s="4" t="s">
+        <v>919</v>
+      </c>
+      <c r="B908" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C908" s="4"/>
+      <c r="D908" s="4"/>
+    </row>
+    <row r="909" spans="1:4">
+      <c r="A909" s="4" t="s">
+        <v>920</v>
+      </c>
+      <c r="B909" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C909" s="4"/>
+      <c r="D909" s="4"/>
+    </row>
+    <row r="910" spans="1:4">
+      <c r="A910" s="4" t="s">
+        <v>921</v>
+      </c>
+      <c r="B910" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C910" s="4"/>
+      <c r="D910" s="4"/>
+    </row>
+    <row r="911" spans="1:4">
+      <c r="A911" s="4" t="s">
+        <v>922</v>
+      </c>
+      <c r="B911" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C911" s="4"/>
+      <c r="D911" s="4"/>
+    </row>
+    <row r="912" spans="1:4">
+      <c r="A912" s="4" t="s">
+        <v>923</v>
+      </c>
+      <c r="B912" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C912" s="4"/>
+      <c r="D912" s="4"/>
+    </row>
+    <row r="913" spans="1:4">
+      <c r="A913" s="4" t="s">
+        <v>924</v>
+      </c>
+      <c r="B913" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C913" s="4"/>
+      <c r="D913" s="4"/>
+    </row>
+    <row r="914" spans="1:4">
+      <c r="A914" s="4" t="s">
+        <v>925</v>
+      </c>
+      <c r="B914" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C914" s="4"/>
+      <c r="D914" s="4"/>
+    </row>
+    <row r="915" spans="1:4">
+      <c r="A915" s="4" t="s">
+        <v>926</v>
+      </c>
+      <c r="B915" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C915" s="4"/>
+      <c r="D915" s="4"/>
+    </row>
+    <row r="916" spans="1:4">
+      <c r="A916" s="4" t="s">
+        <v>927</v>
+      </c>
+      <c r="B916" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C916" s="4"/>
+      <c r="D916" s="4"/>
+    </row>
+    <row r="917" spans="1:4">
+      <c r="A917" s="4" t="s">
+        <v>928</v>
+      </c>
+      <c r="B917" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C917" s="4"/>
+      <c r="D917" s="4"/>
+    </row>
+    <row r="918" spans="1:4">
+      <c r="A918" s="4" t="s">
+        <v>929</v>
+      </c>
+      <c r="B918" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C918" s="4"/>
+      <c r="D918" s="4"/>
+    </row>
+    <row r="919" spans="1:4">
+      <c r="A919" s="4" t="s">
+        <v>930</v>
+      </c>
+      <c r="B919" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C919" s="4"/>
+      <c r="D919" s="4"/>
+    </row>
+    <row r="920" spans="1:4">
+      <c r="A920" s="4" t="s">
+        <v>931</v>
+      </c>
+      <c r="B920" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C920" s="4"/>
+      <c r="D920" s="4"/>
+    </row>
+    <row r="921" spans="1:4">
+      <c r="A921" s="4" t="s">
+        <v>932</v>
+      </c>
+      <c r="B921" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C921" s="4"/>
+      <c r="D921" s="4"/>
+    </row>
+    <row r="922" spans="1:4">
+      <c r="A922" s="4" t="s">
+        <v>933</v>
+      </c>
+      <c r="B922" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C922" s="4"/>
+      <c r="D922" s="4"/>
+    </row>
+    <row r="923" spans="1:4">
+      <c r="A923" s="4" t="s">
+        <v>934</v>
+      </c>
+      <c r="B923" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C923" s="4"/>
+      <c r="D923" s="4"/>
+    </row>
+    <row r="924" spans="1:4">
+      <c r="A924" s="4" t="s">
+        <v>935</v>
+      </c>
+      <c r="B924" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C924" s="4"/>
+      <c r="D924" s="4"/>
+    </row>
+    <row r="925" spans="1:4">
+      <c r="A925" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="B925" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C925" s="4"/>
+      <c r="D925" s="4"/>
+    </row>
+    <row r="926" spans="1:4">
+      <c r="A926" s="4" t="s">
+        <v>937</v>
+      </c>
+      <c r="B926" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C926" s="4"/>
+      <c r="D926" s="4"/>
+    </row>
+    <row r="927" spans="1:4">
+      <c r="A927" s="4" t="s">
+        <v>938</v>
+      </c>
+      <c r="B927" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C927" s="4"/>
+      <c r="D927" s="4"/>
+    </row>
+    <row r="928" spans="1:4">
+      <c r="A928" s="4" t="s">
+        <v>939</v>
+      </c>
+      <c r="B928" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C928" s="4"/>
+      <c r="D928" s="4"/>
+    </row>
+    <row r="929" spans="1:4">
+      <c r="A929" s="4" t="s">
+        <v>940</v>
+      </c>
+      <c r="B929" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C929" s="4"/>
+      <c r="D929" s="4"/>
+    </row>
+    <row r="930" spans="1:4">
+      <c r="A930" s="4" t="s">
+        <v>941</v>
+      </c>
+      <c r="B930" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C930" s="4"/>
+      <c r="D930" s="4"/>
+    </row>
+    <row r="931" spans="1:4">
+      <c r="A931" s="4" t="s">
+        <v>942</v>
+      </c>
+      <c r="B931" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C931" s="4"/>
+      <c r="D931" s="4"/>
+    </row>
+    <row r="932" spans="1:4">
+      <c r="A932" s="4" t="s">
+        <v>943</v>
+      </c>
+      <c r="B932" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C932" s="4"/>
+      <c r="D932" s="4"/>
+    </row>
+    <row r="933" spans="1:4">
+      <c r="A933" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="B933" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C933" s="4"/>
+      <c r="D933" s="4"/>
+    </row>
+    <row r="934" spans="1:4">
+      <c r="A934" s="4" t="s">
+        <v>945</v>
+      </c>
+      <c r="B934" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C934" s="4"/>
+      <c r="D934" s="4"/>
+    </row>
+    <row r="935" spans="1:4">
+      <c r="A935" s="4" t="s">
+        <v>946</v>
+      </c>
+      <c r="B935" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C935" s="4"/>
+      <c r="D935" s="4"/>
+    </row>
+    <row r="936" spans="1:4">
+      <c r="A936" s="4" t="s">
+        <v>947</v>
+      </c>
+      <c r="B936" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C936" s="4"/>
+      <c r="D936" s="4"/>
+    </row>
+    <row r="937" spans="1:4">
+      <c r="A937" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="B937" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C937" s="4"/>
+      <c r="D937" s="4"/>
+    </row>
+    <row r="938" spans="1:4">
+      <c r="A938" s="4" t="s">
+        <v>949</v>
+      </c>
+      <c r="B938" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C938" s="4"/>
+      <c r="D938" s="4"/>
+    </row>
+    <row r="939" spans="1:4">
+      <c r="A939" s="4" t="s">
+        <v>950</v>
+      </c>
+      <c r="B939" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C939" s="4"/>
+      <c r="D939" s="4"/>
+    </row>
+    <row r="940" spans="1:4">
+      <c r="A940" s="4" t="s">
+        <v>951</v>
+      </c>
+      <c r="B940" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C940" s="4"/>
+      <c r="D940" s="4"/>
+    </row>
+    <row r="941" spans="1:4">
+      <c r="A941" s="4" t="s">
+        <v>952</v>
+      </c>
+      <c r="B941" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C941" s="4"/>
+      <c r="D941" s="4"/>
+    </row>
+    <row r="942" spans="1:4">
+      <c r="A942" s="4" t="s">
+        <v>953</v>
+      </c>
+      <c r="B942" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C942" s="4"/>
+      <c r="D942" s="4"/>
+    </row>
+    <row r="943" spans="1:4">
+      <c r="A943" s="4" t="s">
+        <v>954</v>
+      </c>
+      <c r="B943" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C943" s="4"/>
+      <c r="D943" s="4"/>
+    </row>
+    <row r="944" spans="1:4">
+      <c r="A944" s="4" t="s">
+        <v>955</v>
+      </c>
+      <c r="B944" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C944" s="4"/>
+      <c r="D944" s="4"/>
+    </row>
+    <row r="945" spans="1:4">
+      <c r="A945" s="4" t="s">
+        <v>956</v>
+      </c>
+      <c r="B945" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C945" s="4"/>
+      <c r="D945" s="4"/>
+    </row>
+    <row r="946" spans="1:4">
+      <c r="A946" s="4" t="s">
+        <v>957</v>
+      </c>
+      <c r="B946" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C946" s="4"/>
+      <c r="D946" s="4"/>
+    </row>
+    <row r="947" spans="1:4">
+      <c r="A947" s="4" t="s">
+        <v>958</v>
+      </c>
+      <c r="B947" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C947" s="4"/>
+      <c r="D947" s="4"/>
+    </row>
+    <row r="948" spans="1:4">
+      <c r="A948" s="4" t="s">
+        <v>959</v>
+      </c>
+      <c r="B948" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C948" s="4"/>
+      <c r="D948" s="4"/>
+    </row>
+    <row r="949" spans="1:4">
+      <c r="A949" s="4" t="s">
+        <v>960</v>
+      </c>
+      <c r="B949" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C949" s="4"/>
+      <c r="D949" s="4"/>
+    </row>
+    <row r="950" spans="1:4">
+      <c r="A950" s="4" t="s">
+        <v>961</v>
+      </c>
+      <c r="B950" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C950" s="4"/>
+      <c r="D950" s="4"/>
+    </row>
+    <row r="951" spans="1:4">
+      <c r="A951" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="B951" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C951" s="4"/>
+      <c r="D951" s="4"/>
+    </row>
+    <row r="952" spans="1:4">
+      <c r="A952" s="4" t="s">
+        <v>963</v>
+      </c>
+      <c r="B952" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C952" s="4"/>
+      <c r="D952" s="4"/>
+    </row>
+    <row r="953" spans="1:4">
+      <c r="A953" s="4" t="s">
+        <v>964</v>
+      </c>
+      <c r="B953" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C953" s="4"/>
+      <c r="D953" s="4"/>
+    </row>
+    <row r="954" spans="1:4">
+      <c r="A954" s="4" t="s">
+        <v>965</v>
+      </c>
+      <c r="B954" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C954" s="4"/>
+      <c r="D954" s="4"/>
+    </row>
+    <row r="955" spans="1:4">
+      <c r="A955" s="4" t="s">
+        <v>966</v>
+      </c>
+      <c r="B955" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C955" s="4"/>
+      <c r="D955" s="4"/>
+    </row>
+    <row r="956" spans="1:4">
+      <c r="A956" s="4" t="s">
+        <v>967</v>
+      </c>
+      <c r="B956" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C956" s="4"/>
+      <c r="D956" s="4"/>
+    </row>
+    <row r="957" spans="1:4">
+      <c r="A957" s="4" t="s">
+        <v>968</v>
+      </c>
+      <c r="B957" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C957" s="4"/>
+      <c r="D957" s="4"/>
+    </row>
+    <row r="958" spans="1:4">
+      <c r="A958" s="4" t="s">
+        <v>969</v>
+      </c>
+      <c r="B958" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C958" s="4"/>
+      <c r="D958" s="4"/>
+    </row>
+    <row r="959" spans="1:4">
+      <c r="A959" s="4" t="s">
+        <v>970</v>
+      </c>
+      <c r="B959" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C959" s="4"/>
+      <c r="D959" s="4"/>
+    </row>
+    <row r="960" spans="1:4">
+      <c r="A960" s="4" t="s">
+        <v>971</v>
+      </c>
+      <c r="B960" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C960" s="4"/>
+      <c r="D960" s="4"/>
+    </row>
+    <row r="961" spans="1:4">
+      <c r="A961" s="4" t="s">
+        <v>972</v>
+      </c>
+      <c r="B961" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C961" s="4"/>
+      <c r="D961" s="4"/>
+    </row>
+    <row r="962" spans="1:4">
+      <c r="A962" s="4" t="s">
+        <v>973</v>
+      </c>
+      <c r="B962" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C962" s="4"/>
+      <c r="D962" s="4"/>
+    </row>
+    <row r="963" spans="1:4">
+      <c r="A963" s="4" t="s">
+        <v>974</v>
+      </c>
+      <c r="B963" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C963" s="4"/>
+      <c r="D963" s="4"/>
+    </row>
+    <row r="964" spans="1:4">
+      <c r="A964" s="4" t="s">
+        <v>975</v>
+      </c>
+      <c r="B964" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C964" s="4"/>
+      <c r="D964" s="4"/>
+    </row>
+    <row r="965" spans="1:4">
+      <c r="A965" s="4" t="s">
+        <v>976</v>
+      </c>
+      <c r="B965" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C965" s="4"/>
+      <c r="D965" s="4"/>
+    </row>
+    <row r="966" spans="1:4">
+      <c r="A966" s="4" t="s">
+        <v>977</v>
+      </c>
+      <c r="B966" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C966" s="4"/>
+      <c r="D966" s="4"/>
+    </row>
+    <row r="967" spans="1:4">
+      <c r="A967" s="4" t="s">
+        <v>978</v>
+      </c>
+      <c r="B967" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C967" s="4"/>
+      <c r="D967" s="4"/>
+    </row>
+    <row r="968" spans="1:4">
+      <c r="A968" s="4" t="s">
+        <v>979</v>
+      </c>
+      <c r="B968" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C968" s="4"/>
+      <c r="D968" s="4"/>
+    </row>
+    <row r="969" spans="1:4">
+      <c r="A969" s="4" t="s">
+        <v>980</v>
+      </c>
+      <c r="B969" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C969" s="4"/>
+      <c r="D969" s="4"/>
+    </row>
+    <row r="970" spans="1:4">
+      <c r="A970" s="4" t="s">
+        <v>981</v>
+      </c>
+      <c r="B970" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C970" s="4"/>
+      <c r="D970" s="4"/>
+    </row>
+    <row r="971" spans="1:4">
+      <c r="A971" s="4" t="s">
+        <v>982</v>
+      </c>
+      <c r="B971" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C971" s="4"/>
+      <c r="D971" s="4"/>
+    </row>
+    <row r="972" spans="1:4">
+      <c r="A972" s="4" t="s">
+        <v>983</v>
+      </c>
+      <c r="B972" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C972" s="4"/>
+      <c r="D972" s="4"/>
+    </row>
+    <row r="973" spans="1:4">
+      <c r="A973" s="4" t="s">
+        <v>984</v>
+      </c>
+      <c r="B973" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C973" s="4"/>
+      <c r="D973" s="4"/>
+    </row>
+    <row r="974" spans="1:4">
+      <c r="A974" s="4" t="s">
+        <v>985</v>
+      </c>
+      <c r="B974" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C974" s="4"/>
+      <c r="D974" s="4"/>
+    </row>
+    <row r="975" spans="1:4">
+      <c r="A975" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="B975" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C975" s="4"/>
+      <c r="D975" s="4"/>
+    </row>
+    <row r="976" spans="1:4">
+      <c r="A976" s="4" t="s">
+        <v>987</v>
+      </c>
+      <c r="B976" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C976" s="4"/>
+      <c r="D976" s="4"/>
+    </row>
+    <row r="977" spans="1:4">
+      <c r="A977" s="4" t="s">
+        <v>988</v>
+      </c>
+      <c r="B977" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C977" s="4"/>
+      <c r="D977" s="4"/>
+    </row>
+    <row r="978" spans="1:4">
+      <c r="A978" s="4" t="s">
+        <v>989</v>
+      </c>
+      <c r="B978" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C978" s="4"/>
+      <c r="D978" s="4"/>
+    </row>
+    <row r="979" spans="1:4">
+      <c r="A979" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="B979" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C979" s="4"/>
+      <c r="D979" s="4"/>
+    </row>
+    <row r="980" spans="1:4">
+      <c r="A980" s="4" t="s">
+        <v>991</v>
+      </c>
+      <c r="B980" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C980" s="4"/>
+      <c r="D980" s="4"/>
+    </row>
+    <row r="981" spans="1:4">
+      <c r="A981" s="4" t="s">
+        <v>992</v>
+      </c>
+      <c r="B981" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C981" s="4"/>
+      <c r="D981" s="4"/>
+    </row>
+    <row r="982" spans="1:4">
+      <c r="A982" s="4" t="s">
+        <v>993</v>
+      </c>
+      <c r="B982" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C982" s="4"/>
+      <c r="D982" s="4"/>
+    </row>
+    <row r="983" spans="1:4">
+      <c r="A983" s="4" t="s">
+        <v>994</v>
+      </c>
+      <c r="B983" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C983" s="4"/>
+      <c r="D983" s="4"/>
+    </row>
+    <row r="984" spans="1:4">
+      <c r="A984" s="4" t="s">
+        <v>995</v>
+      </c>
+      <c r="B984" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C984" s="4"/>
+      <c r="D984" s="4"/>
+    </row>
+    <row r="985" spans="1:4">
+      <c r="A985" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="B985" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C985" s="4"/>
+      <c r="D985" s="4"/>
+    </row>
+    <row r="986" spans="1:4">
+      <c r="A986" s="4" t="s">
+        <v>997</v>
+      </c>
+      <c r="B986" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C986" s="4"/>
+      <c r="D986" s="4"/>
+    </row>
+    <row r="987" spans="1:4">
+      <c r="A987" s="4" t="s">
+        <v>998</v>
+      </c>
+      <c r="B987" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C987" s="4"/>
+      <c r="D987" s="4"/>
+    </row>
+    <row r="988" spans="1:4">
+      <c r="A988" s="4" t="s">
+        <v>999</v>
+      </c>
+      <c r="B988" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C988" s="4"/>
+      <c r="D988" s="4"/>
+    </row>
+    <row r="989" spans="1:4">
+      <c r="A989" s="4" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B989" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C989" s="4"/>
+      <c r="D989" s="4"/>
+    </row>
+    <row r="990" spans="1:4">
+      <c r="A990" s="4" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B990" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C990" s="4"/>
+      <c r="D990" s="4"/>
+    </row>
+    <row r="991" spans="1:4">
+      <c r="A991" s="4" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B991" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C991" s="4"/>
+      <c r="D991" s="4"/>
+    </row>
+    <row r="992" spans="1:4">
+      <c r="A992" s="4" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B992" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C992" s="4"/>
+      <c r="D992" s="4"/>
+    </row>
+    <row r="993" spans="1:4">
+      <c r="A993" s="4" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B993" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C993" s="4"/>
+      <c r="D993" s="4"/>
+    </row>
+    <row r="994" spans="1:4">
+      <c r="A994" s="4" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B994" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C994" s="4"/>
+      <c r="D994" s="4"/>
+    </row>
+    <row r="995" spans="1:4">
+      <c r="A995" s="4" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B995" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C995" s="4"/>
+      <c r="D995" s="4"/>
+    </row>
+    <row r="996" spans="1:4">
+      <c r="A996" s="4" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B996" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C996" s="4"/>
+      <c r="D996" s="4"/>
+    </row>
+    <row r="997" spans="1:4">
+      <c r="A997" s="4" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B997" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C997" s="4"/>
+      <c r="D997" s="4"/>
+    </row>
+    <row r="998" spans="1:4">
+      <c r="A998" s="4" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B998" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C998" s="4"/>
+      <c r="D998" s="4"/>
+    </row>
+    <row r="999" spans="1:4">
+      <c r="A999" s="4" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B999" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C999" s="4"/>
+      <c r="D999" s="4"/>
+    </row>
+    <row r="1000" spans="1:4">
+      <c r="A1000" s="4" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B1000" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1000" s="4"/>
+      <c r="D1000" s="4"/>
+    </row>
+    <row r="1001" spans="1:4">
+      <c r="A1001" s="4" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B1001" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1001" s="4"/>
+      <c r="D1001" s="4"/>
+    </row>
+    <row r="1002" spans="1:4">
+      <c r="A1002" s="4" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B1002" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1002" s="4"/>
+      <c r="D1002" s="4"/>
+    </row>
+    <row r="1003" spans="1:4">
+      <c r="A1003" s="4" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B1003" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1003" s="4"/>
+      <c r="D1003" s="4"/>
+    </row>
+    <row r="1004" spans="1:4">
+      <c r="A1004" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B1004" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1004" s="4"/>
+      <c r="D1004" s="4"/>
+    </row>
+    <row r="1005" spans="1:4">
+      <c r="A1005" s="4" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B1005" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1005" s="4"/>
+      <c r="D1005" s="4"/>
+    </row>
+    <row r="1006" spans="1:4">
+      <c r="A1006" s="4" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B1006" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1006" s="4"/>
+      <c r="D1006" s="4"/>
+    </row>
+    <row r="1007" spans="1:4">
+      <c r="A1007" s="4" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B1007" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1007" s="4"/>
+      <c r="D1007" s="4"/>
+    </row>
+    <row r="1008" spans="1:4">
+      <c r="A1008" s="4" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B1008" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1008" s="4"/>
+      <c r="D1008" s="4"/>
+    </row>
+    <row r="1009" spans="1:4">
+      <c r="A1009" s="4" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B1009" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1009" s="4"/>
+      <c r="D1009" s="4"/>
+    </row>
+    <row r="1010" spans="1:4">
+      <c r="A1010" s="4" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B1010" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1010" s="4"/>
+      <c r="D1010" s="4"/>
+    </row>
+    <row r="1011" spans="1:4">
+      <c r="A1011" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B1011" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1011" s="4"/>
+      <c r="D1011" s="4"/>
+    </row>
+    <row r="1012" spans="1:4">
+      <c r="A1012" s="4" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B1012" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1012" s="4"/>
+      <c r="D1012" s="4"/>
+    </row>
+    <row r="1013" spans="1:4">
+      <c r="A1013" s="4" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B1013" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1013" s="4"/>
+      <c r="D1013" s="4"/>
+    </row>
+    <row r="1014" spans="1:4">
+      <c r="A1014" s="4" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B1014" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1014" s="4"/>
+      <c r="D1014" s="4"/>
+    </row>
+    <row r="1015" spans="1:4">
+      <c r="A1015" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B1015" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1015" s="4"/>
+      <c r="D1015" s="4"/>
+    </row>
+    <row r="1016" spans="1:4">
+      <c r="A1016" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B1016" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1016" s="4"/>
+      <c r="D1016" s="4"/>
+    </row>
+    <row r="1017" spans="1:4">
+      <c r="A1017" s="4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B1017" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1017" s="4"/>
+      <c r="D1017" s="4"/>
+    </row>
+    <row r="1018" spans="1:4">
+      <c r="A1018" s="4" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B1018" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1018" s="4"/>
+      <c r="D1018" s="4"/>
+    </row>
+    <row r="1019" spans="1:4">
+      <c r="A1019" s="4" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B1019" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1019" s="4"/>
+      <c r="D1019" s="4"/>
+    </row>
+    <row r="1020" spans="1:4">
+      <c r="A1020" s="4" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B1020" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1020" s="4"/>
+      <c r="D1020" s="4"/>
+    </row>
+    <row r="1021" spans="1:4">
+      <c r="A1021" s="4" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B1021" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1021" s="4"/>
+      <c r="D1021" s="4"/>
+    </row>
+    <row r="1022" spans="1:4">
+      <c r="A1022" s="4" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B1022" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1022" s="4"/>
+      <c r="D1022" s="4"/>
+    </row>
+    <row r="1023" spans="1:4">
+      <c r="A1023" s="4" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B1023" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1023" s="4"/>
+      <c r="D1023" s="4"/>
+    </row>
+    <row r="1024" spans="1:4">
+      <c r="A1024" s="4" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B1024" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1024" s="4"/>
+      <c r="D1024" s="4"/>
+    </row>
+    <row r="1025" spans="1:4">
+      <c r="A1025" s="4" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B1025" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1025" s="4"/>
+      <c r="D1025" s="4"/>
+    </row>
+    <row r="1026" spans="1:4">
+      <c r="A1026" s="4" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B1026" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1026" s="4"/>
+      <c r="D1026" s="4"/>
+    </row>
+    <row r="1027" spans="1:4">
+      <c r="A1027" s="4" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B1027" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1027" s="4"/>
+      <c r="D1027" s="4"/>
+    </row>
+    <row r="1028" spans="1:4">
+      <c r="A1028" s="4" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B1028" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1028" s="4"/>
+      <c r="D1028" s="4"/>
+    </row>
+    <row r="1029" spans="1:4">
+      <c r="A1029" s="4" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B1029" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1029" s="4"/>
+      <c r="D1029" s="4"/>
+    </row>
+    <row r="1030" spans="1:4">
+      <c r="A1030" s="4" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B1030" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1030" s="4"/>
+      <c r="D1030" s="4"/>
+    </row>
+    <row r="1031" spans="1:4">
+      <c r="A1031" s="4" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B1031" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1031" s="4"/>
+      <c r="D1031" s="4"/>
+    </row>
+    <row r="1032" spans="1:4">
+      <c r="A1032" s="4" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B1032" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1032" s="4"/>
+      <c r="D1032" s="4"/>
+    </row>
+    <row r="1033" spans="1:4">
+      <c r="A1033" s="4" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B1033" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1033" s="4"/>
+      <c r="D1033" s="4"/>
+    </row>
+    <row r="1034" spans="1:4">
+      <c r="A1034" s="4" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B1034" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1034" s="4"/>
+      <c r="D1034" s="4"/>
+    </row>
+    <row r="1035" spans="1:4">
+      <c r="A1035" s="4" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B1035" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1035" s="4"/>
+      <c r="D1035" s="4"/>
+    </row>
+    <row r="1036" spans="1:4">
+      <c r="A1036" s="4" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B1036" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1036" s="4"/>
+      <c r="D1036" s="4"/>
+    </row>
+    <row r="1037" spans="1:4">
+      <c r="A1037" s="4" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B1037" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1037" s="4"/>
+      <c r="D1037" s="4"/>
+    </row>
+    <row r="1038" spans="1:4">
+      <c r="A1038" s="4" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B1038" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1038" s="4"/>
+      <c r="D1038" s="4"/>
+    </row>
+    <row r="1039" spans="1:4">
+      <c r="A1039" s="4" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B1039" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1039" s="4"/>
+      <c r="D1039" s="4"/>
+    </row>
+    <row r="1040" spans="1:4">
+      <c r="A1040" s="4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B1040" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1040" s="4"/>
+      <c r="D1040" s="4"/>
+    </row>
+    <row r="1041" spans="1:4">
+      <c r="A1041" s="4" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B1041" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1041" s="4"/>
+      <c r="D1041" s="4"/>
+    </row>
+    <row r="1042" spans="1:4">
+      <c r="A1042" s="4" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B1042" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1042" s="4"/>
+      <c r="D1042" s="4"/>
+    </row>
+    <row r="1043" spans="1:4">
+      <c r="A1043" s="4" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B1043" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1043" s="4"/>
+      <c r="D1043" s="4"/>
+    </row>
+    <row r="1044" spans="1:4">
+      <c r="A1044" s="4" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B1044" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1044" s="4"/>
+      <c r="D1044" s="4"/>
+    </row>
+    <row r="1045" spans="1:4">
+      <c r="A1045" s="4" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B1045" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1045" s="4"/>
+      <c r="D1045" s="4"/>
+    </row>
+    <row r="1046" spans="1:4">
+      <c r="A1046" s="4" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B1046" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1046" s="4"/>
+      <c r="D1046" s="4"/>
+    </row>
+    <row r="1047" spans="1:4">
+      <c r="A1047" s="4" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B1047" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1047" s="4"/>
+      <c r="D1047" s="4"/>
+    </row>
+    <row r="1048" spans="1:4">
+      <c r="A1048" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B1048" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1048" s="4"/>
+      <c r="D1048" s="4"/>
+    </row>
+    <row r="1049" spans="1:4">
+      <c r="A1049" s="4" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B1049" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1049" s="4"/>
+      <c r="D1049" s="4"/>
+    </row>
+    <row r="1050" spans="1:4">
+      <c r="A1050" s="4" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B1050" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1050" s="4"/>
+      <c r="D1050" s="4"/>
+    </row>
+    <row r="1051" spans="1:4">
+      <c r="A1051" s="4" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B1051" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1051" s="4"/>
+      <c r="D1051" s="4"/>
+    </row>
+    <row r="1052" spans="1:4">
+      <c r="A1052" s="4" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B1052" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1052" s="4"/>
+      <c r="D1052" s="4"/>
+    </row>
+    <row r="1053" spans="1:4">
+      <c r="A1053" s="4" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B1053" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1053" s="4"/>
+      <c r="D1053" s="4"/>
+    </row>
+    <row r="1054" spans="1:4">
+      <c r="A1054" s="4" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B1054" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1054" s="4"/>
+      <c r="D1054" s="4"/>
+    </row>
+    <row r="1055" spans="1:4">
+      <c r="A1055" s="4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1055" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1055" s="4"/>
+      <c r="D1055" s="4"/>
+    </row>
+    <row r="1056" spans="1:4">
+      <c r="A1056" s="4" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B1056" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1056" s="4"/>
+      <c r="D1056" s="4"/>
+    </row>
+    <row r="1057" spans="1:4">
+      <c r="A1057" s="4" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B1057" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1057" s="4"/>
+      <c r="D1057" s="4"/>
+    </row>
+    <row r="1058" spans="1:4">
+      <c r="A1058" s="4" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B1058" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1058" s="4"/>
+      <c r="D1058" s="4"/>
+    </row>
+    <row r="1059" spans="1:4">
+      <c r="A1059" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B1059" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1059" s="4"/>
+      <c r="D1059" s="4"/>
+    </row>
+    <row r="1060" spans="1:4">
+      <c r="A1060" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B1060" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1060" s="4"/>
+      <c r="D1060" s="4"/>
+    </row>
+    <row r="1061" spans="1:4">
+      <c r="A1061" s="4" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1061" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1061" s="4"/>
+      <c r="D1061" s="4"/>
+    </row>
+    <row r="1062" spans="1:4">
+      <c r="A1062" s="4" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B1062" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1062" s="4"/>
+      <c r="D1062" s="4"/>
+    </row>
+    <row r="1063" spans="1:4">
+      <c r="A1063" s="4" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B1063" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1063" s="4"/>
+      <c r="D1063" s="4"/>
+    </row>
+    <row r="1064" spans="1:4">
+      <c r="A1064" s="4" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B1064" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1064" s="4"/>
+      <c r="D1064" s="4"/>
+    </row>
+    <row r="1065" spans="1:4">
+      <c r="A1065" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1065" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1065" s="4"/>
+      <c r="D1065" s="4"/>
+    </row>
+    <row r="1066" spans="1:4">
+      <c r="A1066" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B1066" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1066" s="4"/>
+      <c r="D1066" s="4"/>
+    </row>
+    <row r="1067" spans="1:4">
+      <c r="A1067" s="4" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B1067" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1067" s="4"/>
+      <c r="D1067" s="4"/>
+    </row>
+    <row r="1068" spans="1:4">
+      <c r="A1068" s="4" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B1068" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1068" s="4"/>
+      <c r="D1068" s="4"/>
+    </row>
+    <row r="1069" spans="1:4">
+      <c r="A1069" s="4" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B1069" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1069" s="4"/>
+      <c r="D1069" s="4"/>
+    </row>
+    <row r="1070" spans="1:4">
+      <c r="A1070" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B1070" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1070" s="4"/>
+      <c r="D1070" s="4"/>
+    </row>
+    <row r="1071" spans="1:4">
+      <c r="A1071" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B1071" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1071" s="4"/>
+      <c r="D1071" s="4"/>
+    </row>
+    <row r="1072" spans="1:4">
+      <c r="A1072" s="4" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B1072" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1072" s="4"/>
+      <c r="D1072" s="4"/>
+    </row>
+    <row r="1073" spans="1:4">
+      <c r="A1073" s="4" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B1073" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1073" s="4"/>
+      <c r="D1073" s="4"/>
+    </row>
+    <row r="1074" spans="1:4">
+      <c r="A1074" s="4" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B1074" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1074" s="4"/>
+      <c r="D1074" s="4"/>
+    </row>
+    <row r="1075" spans="1:4">
+      <c r="A1075" s="4" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B1075" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1075" s="4"/>
+      <c r="D1075" s="4"/>
+    </row>
+    <row r="1076" spans="1:4">
+      <c r="A1076" s="4" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B1076" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1076" s="4"/>
+      <c r="D1076" s="4"/>
+    </row>
+    <row r="1077" spans="1:4">
+      <c r="A1077" s="4" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B1077" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1077" s="4"/>
+      <c r="D1077" s="4"/>
+    </row>
+    <row r="1078" spans="1:4">
+      <c r="A1078" s="4" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B1078" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1078" s="4"/>
+      <c r="D1078" s="4"/>
+    </row>
+    <row r="1079" spans="1:4">
+      <c r="A1079" s="4" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B1079" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1079" s="4"/>
+      <c r="D1079" s="4"/>
+    </row>
+    <row r="1080" spans="1:4">
+      <c r="A1080" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B1080" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1080" s="4"/>
+      <c r="D1080" s="4"/>
+    </row>
+    <row r="1081" spans="1:4">
+      <c r="A1081" s="4" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B1081" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1081" s="4"/>
+      <c r="D1081" s="4"/>
+    </row>
+    <row r="1082" spans="1:4">
+      <c r="A1082" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B1082" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1082" s="4"/>
+      <c r="D1082" s="4"/>
+    </row>
+    <row r="1083" spans="1:4">
+      <c r="A1083" s="4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B1083" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1083" s="4"/>
+      <c r="D1083" s="4"/>
+    </row>
+    <row r="1084" spans="1:4">
+      <c r="A1084" s="4" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B1084" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1084" s="4"/>
+      <c r="D1084" s="4"/>
+    </row>
+    <row r="1085" spans="1:4">
+      <c r="A1085" s="4" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B1085" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1085" s="4"/>
+      <c r="D1085" s="4"/>
+    </row>
+    <row r="1086" spans="1:4">
+      <c r="A1086" s="4" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B1086" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1086" s="4"/>
+      <c r="D1086" s="4"/>
+    </row>
+    <row r="1087" spans="1:4">
+      <c r="A1087" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B1087" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1087" s="4"/>
+      <c r="D1087" s="4"/>
+    </row>
+    <row r="1088" spans="1:4">
+      <c r="A1088" s="4" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B1088" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1088" s="4"/>
+      <c r="D1088" s="4"/>
+    </row>
+    <row r="1089" spans="1:4">
+      <c r="A1089" s="4" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B1089" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1089" s="4"/>
+      <c r="D1089" s="4"/>
+    </row>
+    <row r="1090" spans="1:4">
+      <c r="A1090" s="4" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B1090" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1090" s="4"/>
+      <c r="D1090" s="4"/>
+    </row>
+    <row r="1091" spans="1:4">
+      <c r="A1091" s="4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B1091" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1091" s="4"/>
+      <c r="D1091" s="4"/>
+    </row>
+    <row r="1092" spans="1:4">
+      <c r="A1092" s="4" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B1092" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1092" s="4"/>
+      <c r="D1092" s="4"/>
+    </row>
+    <row r="1093" spans="1:4">
+      <c r="A1093" s="4" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B1093" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1093" s="4"/>
+      <c r="D1093" s="4"/>
+    </row>
+    <row r="1094" spans="1:4">
+      <c r="A1094" s="4" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B1094" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1094" s="4"/>
+      <c r="D1094" s="4"/>
+    </row>
+    <row r="1095" spans="1:4">
+      <c r="A1095" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B1095" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1095" s="4"/>
+      <c r="D1095" s="4"/>
+    </row>
+    <row r="1096" spans="1:4">
+      <c r="A1096" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1096" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1096" s="4"/>
+      <c r="D1096" s="4"/>
+    </row>
+    <row r="1097" spans="1:4">
+      <c r="A1097" s="4" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B1097" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1097" s="4"/>
+      <c r="D1097" s="4"/>
+    </row>
+    <row r="1098" spans="1:4">
+      <c r="A1098" s="4" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B1098" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1098" s="4"/>
+      <c r="D1098" s="4"/>
+    </row>
+    <row r="1099" spans="1:4">
+      <c r="A1099" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B1099" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1099" s="4"/>
+      <c r="D1099" s="4"/>
+    </row>
+    <row r="1100" spans="1:4">
+      <c r="A1100" s="4" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B1100" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1100" s="4"/>
+      <c r="D1100" s="4"/>
+    </row>
+    <row r="1101" spans="1:4">
+      <c r="A1101" s="4" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B1101" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1101" s="4"/>
+      <c r="D1101" s="4"/>
+    </row>
+    <row r="1102" spans="1:4">
+      <c r="A1102" s="4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B1102" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1102" s="4"/>
+      <c r="D1102" s="4"/>
+    </row>
+    <row r="1103" spans="1:4">
+      <c r="A1103" s="4" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B1103" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1103" s="4"/>
+      <c r="D1103" s="4"/>
+    </row>
+    <row r="1104" spans="1:4">
+      <c r="A1104" s="4" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B1104" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1104" s="4"/>
+      <c r="D1104" s="4"/>
+    </row>
+    <row r="1105" spans="1:4">
+      <c r="A1105" s="4" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B1105" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1105" s="4"/>
+      <c r="D1105" s="4"/>
+    </row>
+    <row r="1106" spans="1:4">
+      <c r="A1106" s="4" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B1106" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1106" s="4"/>
+      <c r="D1106" s="4"/>
+    </row>
+    <row r="1107" spans="1:4">
+      <c r="A1107" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B1107" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1107" s="4"/>
+      <c r="D1107" s="4"/>
+    </row>
+    <row r="1108" spans="1:4">
+      <c r="A1108" s="4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B1108" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1108" s="4"/>
+      <c r="D1108" s="4"/>
+    </row>
+    <row r="1109" spans="1:4">
+      <c r="A1109" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B1109" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1109" s="4"/>
+      <c r="D1109" s="4"/>
+    </row>
+    <row r="1110" spans="1:4">
+      <c r="A1110" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B1110" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1110" s="4"/>
+      <c r="D1110" s="4"/>
+    </row>
+    <row r="1111" spans="1:4">
+      <c r="A1111" s="4" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B1111" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1111" s="4"/>
+      <c r="D1111" s="4"/>
+    </row>
+    <row r="1112" spans="1:4">
+      <c r="A1112" s="4" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B1112" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1112" s="4"/>
+      <c r="D1112" s="4"/>
+    </row>
+    <row r="1113" spans="1:4">
+      <c r="A1113" s="4" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B1113" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1113" s="4"/>
+      <c r="D1113" s="4"/>
+    </row>
+    <row r="1114" spans="1:4">
+      <c r="A1114" s="4" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B1114" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1114" s="4"/>
+      <c r="D1114" s="4"/>
+    </row>
+    <row r="1115" spans="1:4">
+      <c r="A1115" s="4" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B1115" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1115" s="4"/>
+      <c r="D1115" s="4"/>
+    </row>
+    <row r="1116" spans="1:4">
+      <c r="A1116" s="4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B1116" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1116" s="4"/>
+      <c r="D1116" s="4"/>
+    </row>
+    <row r="1117" spans="1:4">
+      <c r="A1117" s="4" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B1117" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1117" s="4"/>
+      <c r="D1117" s="4"/>
+    </row>
+    <row r="1118" spans="1:4">
+      <c r="A1118" s="4" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B1118" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1118" s="4"/>
+      <c r="D1118" s="4"/>
+    </row>
+    <row r="1119" spans="1:4">
+      <c r="A1119" s="4" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B1119" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1119" s="4"/>
+      <c r="D1119" s="4"/>
+    </row>
+    <row r="1120" spans="1:4">
+      <c r="A1120" s="4" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B1120" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1120" s="4"/>
+      <c r="D1120" s="4"/>
+    </row>
+    <row r="1121" spans="1:4">
+      <c r="A1121" s="4" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B1121" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1121" s="4"/>
+      <c r="D1121" s="4"/>
+    </row>
+    <row r="1122" spans="1:4">
+      <c r="A1122" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B1122" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1122" s="4"/>
+      <c r="D1122" s="4"/>
+    </row>
+    <row r="1123" spans="1:4">
+      <c r="A1123" s="4" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B1123" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1123" s="4"/>
+      <c r="D1123" s="4"/>
+    </row>
+    <row r="1124" spans="1:4">
+      <c r="A1124" s="4" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B1124" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1124" s="4"/>
+      <c r="D1124" s="4"/>
+    </row>
+    <row r="1125" spans="1:4">
+      <c r="A1125" s="4" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B1125" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1125" s="4"/>
+      <c r="D1125" s="4"/>
+    </row>
+    <row r="1126" spans="1:4">
+      <c r="A1126" s="4" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B1126" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1126" s="4"/>
+      <c r="D1126" s="4"/>
+    </row>
+    <row r="1127" spans="1:4">
+      <c r="A1127" s="4" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B1127" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1127" s="4"/>
+      <c r="D1127" s="4"/>
+    </row>
+    <row r="1128" spans="1:4">
+      <c r="A1128" s="4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B1128" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1128" s="4"/>
+      <c r="D1128" s="4"/>
+    </row>
+    <row r="1129" spans="1:4">
+      <c r="A1129" s="4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B1129" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1129" s="4"/>
+      <c r="D1129" s="4"/>
+    </row>
+    <row r="1130" spans="1:4">
+      <c r="A1130" s="4" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B1130" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1130" s="4"/>
+      <c r="D1130" s="4"/>
+    </row>
+    <row r="1131" spans="1:4">
+      <c r="A1131" s="4" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B1131" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1131" s="4"/>
+      <c r="D1131" s="4"/>
+    </row>
+    <row r="1132" spans="1:4">
+      <c r="A1132" s="4" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B1132" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1132" s="4"/>
+      <c r="D1132" s="4"/>
+    </row>
+    <row r="1133" spans="1:4">
+      <c r="A1133" s="4" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B1133" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1133" s="4"/>
+      <c r="D1133" s="4"/>
+    </row>
+    <row r="1134" spans="1:4">
+      <c r="A1134" s="4" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B1134" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1134" s="4"/>
+      <c r="D1134" s="4"/>
+    </row>
+    <row r="1135" spans="1:4">
+      <c r="A1135" s="4" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B1135" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1135" s="4"/>
+      <c r="D1135" s="4"/>
+    </row>
+    <row r="1136" spans="1:4">
+      <c r="A1136" s="4" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B1136" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1136" s="4"/>
+      <c r="D1136" s="4"/>
+    </row>
+    <row r="1137" spans="1:4">
+      <c r="A1137" s="4" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B1137" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1137" s="4"/>
+      <c r="D1137" s="4"/>
+    </row>
+    <row r="1138" spans="1:4">
+      <c r="A1138" s="4" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B1138" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1138" s="4"/>
+      <c r="D1138" s="4"/>
+    </row>
+    <row r="1139" spans="1:4">
+      <c r="A1139" s="4" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B1139" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1139" s="4"/>
+      <c r="D1139" s="4"/>
+    </row>
+    <row r="1140" spans="1:4">
+      <c r="A1140" s="4" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B1140" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1140" s="4"/>
+      <c r="D1140" s="4"/>
+    </row>
+    <row r="1141" spans="1:4">
+      <c r="A1141" s="4" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B1141" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1141" s="4"/>
+      <c r="D1141" s="4"/>
+    </row>
+    <row r="1142" spans="1:4">
+      <c r="A1142" s="4" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B1142" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1142" s="4"/>
+      <c r="D1142" s="4"/>
+    </row>
+    <row r="1143" spans="1:4">
+      <c r="A1143" s="4" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B1143" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1143" s="4"/>
+      <c r="D1143" s="4"/>
+    </row>
+    <row r="1144" spans="1:4">
+      <c r="A1144" s="4" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B1144" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1144" s="4"/>
+      <c r="D1144" s="4"/>
+    </row>
+    <row r="1145" spans="1:4">
+      <c r="A1145" s="4" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B1145" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1145" s="4"/>
+      <c r="D1145" s="4"/>
+    </row>
+    <row r="1146" spans="1:4">
+      <c r="A1146" s="4" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B1146" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1146" s="4"/>
+      <c r="D1146" s="4"/>
+    </row>
+    <row r="1147" spans="1:4">
+      <c r="A1147" s="4" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B1147" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1147" s="4"/>
+      <c r="D1147" s="4"/>
+    </row>
+    <row r="1148" spans="1:4">
+      <c r="A1148" s="4" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B1148" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1148" s="4"/>
+      <c r="D1148" s="4"/>
+    </row>
+    <row r="1149" spans="1:4">
+      <c r="A1149" s="4" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B1149" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1149" s="4"/>
+      <c r="D1149" s="4"/>
+    </row>
+    <row r="1150" spans="1:4">
+      <c r="A1150" s="4" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B1150" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1150" s="4"/>
+      <c r="D1150" s="4"/>
+    </row>
+    <row r="1151" spans="1:4">
+      <c r="A1151" s="4" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B1151" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1151" s="4"/>
+      <c r="D1151" s="4"/>
+    </row>
+    <row r="1152" spans="1:4">
+      <c r="A1152" s="4" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B1152" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1152" s="4"/>
+      <c r="D1152" s="4"/>
+    </row>
+    <row r="1153" spans="1:4">
+      <c r="A1153" s="4" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B1153" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1153" s="4"/>
+      <c r="D1153" s="4"/>
+    </row>
+    <row r="1154" spans="1:4">
+      <c r="A1154" s="4" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B1154" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1154" s="4"/>
+      <c r="D1154" s="4"/>
+    </row>
+    <row r="1155" spans="1:4">
+      <c r="A1155" s="4" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B1155" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1155" s="4"/>
+      <c r="D1155" s="4"/>
+    </row>
+    <row r="1156" spans="1:4">
+      <c r="A1156" s="4" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B1156" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1156" s="4"/>
+      <c r="D1156" s="4"/>
+    </row>
+    <row r="1157" spans="1:4">
+      <c r="A1157" s="4" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B1157" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1157" s="4"/>
+      <c r="D1157" s="4"/>
+    </row>
+    <row r="1158" spans="1:4">
+      <c r="A1158" s="4" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B1158" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1158" s="4"/>
+      <c r="D1158" s="4"/>
+    </row>
+    <row r="1159" spans="1:4">
+      <c r="A1159" s="4" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B1159" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1159" s="4"/>
+      <c r="D1159" s="4"/>
+    </row>
+    <row r="1160" spans="1:4">
+      <c r="A1160" s="4" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B1160" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1160" s="4"/>
+      <c r="D1160" s="4"/>
+    </row>
+    <row r="1161" spans="1:4">
+      <c r="A1161" s="4" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B1161" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1161" s="4"/>
+      <c r="D1161" s="4"/>
+    </row>
+    <row r="1162" spans="1:4">
+      <c r="A1162" s="4" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B1162" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1162" s="4"/>
+      <c r="D1162" s="4"/>
+    </row>
+    <row r="1163" spans="1:4">
+      <c r="A1163" s="4" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B1163" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1163" s="4"/>
+      <c r="D1163" s="4"/>
+    </row>
+    <row r="1164" spans="1:4">
+      <c r="A1164" s="4" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B1164" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1164" s="4"/>
+      <c r="D1164" s="4"/>
+    </row>
+    <row r="1165" spans="1:4">
+      <c r="A1165" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B1165" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1165" s="4"/>
+      <c r="D1165" s="4"/>
+    </row>
+    <row r="1166" spans="1:4">
+      <c r="A1166" s="4" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B1166" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1166" s="4"/>
+      <c r="D1166" s="4"/>
+    </row>
+    <row r="1167" spans="1:4">
+      <c r="A1167" s="4" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B1167" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1167" s="4"/>
+      <c r="D1167" s="4"/>
+    </row>
+    <row r="1168" spans="1:4">
+      <c r="A1168" s="4" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B1168" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1168" s="4"/>
+      <c r="D1168" s="4"/>
+    </row>
+    <row r="1169" spans="1:4">
+      <c r="A1169" s="4" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B1169" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1169" s="4"/>
+      <c r="D1169" s="4"/>
+    </row>
+    <row r="1170" spans="1:4">
+      <c r="A1170" s="4" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B1170" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1170" s="4"/>
+      <c r="D1170" s="4"/>
+    </row>
+    <row r="1171" spans="1:4">
+      <c r="A1171" s="4" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B1171" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1171" s="4"/>
+      <c r="D1171" s="4"/>
+    </row>
+    <row r="1172" spans="1:4">
+      <c r="A1172" s="4" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B1172" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1172" s="4"/>
+      <c r="D1172" s="4"/>
+    </row>
+    <row r="1173" spans="1:4">
+      <c r="A1173" s="4" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B1173" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1173" s="4"/>
+      <c r="D1173" s="4"/>
+    </row>
+    <row r="1174" spans="1:4">
+      <c r="A1174" s="4" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B1174" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1174" s="4"/>
+      <c r="D1174" s="4"/>
+    </row>
+    <row r="1175" spans="1:4">
+      <c r="A1175" s="4" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B1175" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1175" s="4"/>
+      <c r="D1175" s="4"/>
+    </row>
+    <row r="1176" spans="1:4">
+      <c r="A1176" s="4" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B1176" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1176" s="4"/>
+      <c r="D1176" s="4"/>
+    </row>
+    <row r="1177" spans="1:4">
+      <c r="A1177" s="4" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B1177" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1177" s="4"/>
+      <c r="D1177" s="4"/>
+    </row>
+    <row r="1178" spans="1:4">
+      <c r="A1178" s="4" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B1178" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1178" s="4"/>
+      <c r="D1178" s="4"/>
+    </row>
+    <row r="1179" spans="1:4">
+      <c r="A1179" s="4" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B1179" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1179" s="4"/>
+      <c r="D1179" s="4"/>
+    </row>
+    <row r="1180" spans="1:4">
+      <c r="A1180" s="4" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B1180" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1180" s="4"/>
+      <c r="D1180" s="4"/>
+    </row>
+    <row r="1181" spans="1:4">
+      <c r="A1181" s="4" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B1181" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1181" s="4"/>
+      <c r="D1181" s="4"/>
+    </row>
+    <row r="1182" spans="1:4">
+      <c r="A1182" s="4" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B1182" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1182" s="4"/>
+      <c r="D1182" s="4"/>
+    </row>
+    <row r="1183" spans="1:4">
+      <c r="A1183" s="4" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B1183" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1183" s="4"/>
+      <c r="D1183" s="4"/>
+    </row>
+    <row r="1184" spans="1:4">
+      <c r="A1184" s="4" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B1184" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1184" s="4"/>
+      <c r="D1184" s="4"/>
+    </row>
+    <row r="1185" spans="1:4">
+      <c r="A1185" s="4" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B1185" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1185" s="4"/>
+      <c r="D1185" s="4"/>
+    </row>
+    <row r="1186" spans="1:4">
+      <c r="A1186" s="4" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B1186" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1186" s="4"/>
+      <c r="D1186" s="4"/>
+    </row>
+    <row r="1187" spans="1:4">
+      <c r="A1187" s="4" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B1187" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1187" s="4"/>
+      <c r="D1187" s="4"/>
+    </row>
+    <row r="1188" spans="1:4">
+      <c r="A1188" s="4" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B1188" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1188" s="4"/>
+      <c r="D1188" s="4"/>
+    </row>
+    <row r="1189" spans="1:4">
+      <c r="A1189" s="4" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B1189" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1189" s="4"/>
+      <c r="D1189" s="4"/>
+    </row>
+    <row r="1190" spans="1:4">
+      <c r="A1190" s="4" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B1190" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1190" s="4"/>
+      <c r="D1190" s="4"/>
+    </row>
+    <row r="1191" spans="1:4">
+      <c r="A1191" s="4" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B1191" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1191" s="4"/>
+      <c r="D1191" s="4"/>
+    </row>
+    <row r="1192" spans="1:4">
+      <c r="A1192" s="4" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B1192" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1192" s="4"/>
+      <c r="D1192" s="4"/>
+    </row>
+    <row r="1193" spans="1:4">
+      <c r="A1193" s="4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B1193" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1193" s="4"/>
+      <c r="D1193" s="4"/>
+    </row>
+    <row r="1194" spans="1:4">
+      <c r="A1194" s="4" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B1194" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1194" s="4"/>
+      <c r="D1194" s="4"/>
+    </row>
+    <row r="1195" spans="1:4">
+      <c r="A1195" s="4" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B1195" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1195" s="4"/>
+      <c r="D1195" s="4"/>
+    </row>
+    <row r="1196" spans="1:4">
+      <c r="A1196" s="4" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B1196" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1196" s="4"/>
+      <c r="D1196" s="4"/>
+    </row>
+    <row r="1197" spans="1:4">
+      <c r="A1197" s="4" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B1197" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1197" s="4"/>
+      <c r="D1197" s="4"/>
+    </row>
+    <row r="1198" spans="1:4">
+      <c r="A1198" s="4" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B1198" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1198" s="4"/>
+      <c r="D1198" s="4"/>
+    </row>
+    <row r="1199" spans="1:4">
+      <c r="A1199" s="4" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B1199" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1199" s="4"/>
+      <c r="D1199" s="4"/>
+    </row>
+    <row r="1200" spans="1:4">
+      <c r="A1200" s="4" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B1200" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1200" s="4"/>
+      <c r="D1200" s="4"/>
+    </row>
+    <row r="1201" spans="1:4">
+      <c r="A1201" s="4" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B1201" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1201" s="4"/>
+      <c r="D1201" s="4"/>
+    </row>
+    <row r="1202" spans="1:4">
+      <c r="A1202" s="4" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B1202" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1202" s="4"/>
+      <c r="D1202" s="4"/>
+    </row>
+    <row r="1203" spans="1:4">
+      <c r="A1203" s="4" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B1203" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1203" s="4"/>
+      <c r="D1203" s="4"/>
+    </row>
+    <row r="1204" spans="1:4">
+      <c r="A1204" s="4" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B1204" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1204" s="4"/>
+      <c r="D1204" s="4"/>
+    </row>
+    <row r="1205" spans="1:4">
+      <c r="A1205" s="4" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B1205" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1205" s="4"/>
+      <c r="D1205" s="4"/>
+    </row>
+    <row r="1206" spans="1:4">
+      <c r="A1206" s="4" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B1206" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1206" s="4"/>
+      <c r="D1206" s="4"/>
+    </row>
+    <row r="1207" spans="1:4">
+      <c r="A1207" s="4" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1207" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1207" s="4"/>
+      <c r="D1207" s="4"/>
+    </row>
+    <row r="1208" spans="1:4">
+      <c r="A1208" s="4" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B1208" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1208" s="4"/>
+      <c r="D1208" s="4"/>
+    </row>
+    <row r="1209" spans="1:4">
+      <c r="A1209" s="4" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B1209" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1209" s="4"/>
+      <c r="D1209" s="4"/>
+    </row>
+    <row r="1210" spans="1:4">
+      <c r="A1210" s="4" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B1210" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1210" s="4"/>
+      <c r="D1210" s="4"/>
+    </row>
+    <row r="1211" spans="1:4">
+      <c r="A1211" s="4" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B1211" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1211" s="4"/>
+      <c r="D1211" s="4"/>
+    </row>
+    <row r="1212" spans="1:4">
+      <c r="A1212" s="4" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B1212" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1212" s="4"/>
+      <c r="D1212" s="4"/>
+    </row>
+    <row r="1213" spans="1:4">
+      <c r="A1213" s="4" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B1213" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1213" s="4"/>
+      <c r="D1213" s="4"/>
+    </row>
+    <row r="1214" spans="1:4">
+      <c r="A1214" s="4" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B1214" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1214" s="4"/>
+      <c r="D1214" s="4"/>
+    </row>
+    <row r="1215" spans="1:4">
+      <c r="A1215" s="4" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B1215" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1215" s="4"/>
+      <c r="D1215" s="4"/>
+    </row>
+    <row r="1216" spans="1:4">
+      <c r="A1216" s="4" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B1216" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1216" s="4"/>
+      <c r="D1216" s="4"/>
+    </row>
+    <row r="1217" spans="1:4">
+      <c r="A1217" s="4" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B1217" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1217" s="4"/>
+      <c r="D1217" s="4"/>
+    </row>
+    <row r="1218" spans="1:4">
+      <c r="A1218" s="4" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B1218" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1218" s="4"/>
+      <c r="D1218" s="4"/>
+    </row>
+    <row r="1219" spans="1:4">
+      <c r="A1219" s="4" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B1219" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1219" s="4"/>
+      <c r="D1219" s="4"/>
+    </row>
+    <row r="1220" spans="1:4">
+      <c r="A1220" s="4" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B1220" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1220" s="4"/>
+      <c r="D1220" s="4"/>
+    </row>
+    <row r="1221" spans="1:4">
+      <c r="A1221" s="4" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B1221" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1221" s="4"/>
+      <c r="D1221" s="4"/>
+    </row>
+    <row r="1222" spans="1:4">
+      <c r="A1222" s="4" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B1222" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1222" s="4"/>
+      <c r="D1222" s="4"/>
+    </row>
+    <row r="1223" spans="1:4">
+      <c r="A1223" s="4" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B1223" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1223" s="4"/>
+      <c r="D1223" s="4"/>
+    </row>
+    <row r="1224" spans="1:4">
+      <c r="A1224" s="4" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B1224" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1224" s="4"/>
+      <c r="D1224" s="4"/>
+    </row>
+    <row r="1225" spans="1:4">
+      <c r="A1225" s="4" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B1225" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1225" s="4"/>
+      <c r="D1225" s="4"/>
+    </row>
+    <row r="1226" spans="1:4">
+      <c r="A1226" s="4" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B1226" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1226" s="4"/>
+      <c r="D1226" s="4"/>
+    </row>
+    <row r="1227" spans="1:4">
+      <c r="A1227" s="4" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B1227" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1227" s="4"/>
+      <c r="D1227" s="4"/>
+    </row>
+    <row r="1228" spans="1:4">
+      <c r="A1228" s="4" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B1228" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1228" s="4"/>
+      <c r="D1228" s="4"/>
+    </row>
+    <row r="1229" spans="1:4">
+      <c r="A1229" s="4" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B1229" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1229" s="4"/>
+      <c r="D1229" s="4"/>
+    </row>
+    <row r="1230" spans="1:4">
+      <c r="A1230" s="4" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B1230" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1230" s="4"/>
+      <c r="D1230" s="4"/>
+    </row>
+    <row r="1231" spans="1:4">
+      <c r="A1231" s="4" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B1231" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1231" s="4"/>
+      <c r="D1231" s="4"/>
+    </row>
+    <row r="1232" spans="1:4">
+      <c r="A1232" s="4" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B1232" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1232" s="4"/>
+      <c r="D1232" s="4"/>
+    </row>
+    <row r="1233" spans="1:4">
+      <c r="A1233" s="4" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B1233" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1233" s="4"/>
+      <c r="D1233" s="4"/>
+    </row>
+    <row r="1234" spans="1:4">
+      <c r="A1234" s="4" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B1234" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1234" s="4"/>
+      <c r="D1234" s="4"/>
+    </row>
+    <row r="1235" spans="1:4">
+      <c r="A1235" s="4" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B1235" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1235" s="4"/>
+      <c r="D1235" s="4"/>
+    </row>
+    <row r="1236" spans="1:4">
+      <c r="A1236" s="4" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B1236" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1236" s="4"/>
+      <c r="D1236" s="4"/>
+    </row>
+    <row r="1237" spans="1:4">
+      <c r="A1237" s="4" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B1237" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1237" s="4"/>
+      <c r="D1237" s="4"/>
+    </row>
+    <row r="1238" spans="1:4">
+      <c r="A1238" s="4" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B1238" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1238" s="4"/>
+      <c r="D1238" s="4"/>
+    </row>
+    <row r="1239" spans="1:4">
+      <c r="A1239" s="4" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B1239" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1239" s="4"/>
+      <c r="D1239" s="4"/>
+    </row>
+    <row r="1240" spans="1:4">
+      <c r="A1240" s="4" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B1240" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1240" s="4"/>
+      <c r="D1240" s="4"/>
+    </row>
+    <row r="1241" spans="1:4">
+      <c r="A1241" s="4" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B1241" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1241" s="4"/>
+      <c r="D1241" s="4"/>
+    </row>
+    <row r="1242" spans="1:4">
+      <c r="A1242" s="4" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B1242" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1242" s="4"/>
+      <c r="D1242" s="4"/>
+    </row>
+    <row r="1243" spans="1:4">
+      <c r="A1243" s="4" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B1243" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1243" s="4"/>
+      <c r="D1243" s="4"/>
+    </row>
+    <row r="1244" spans="1:4">
+      <c r="A1244" s="4" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B1244" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1244" s="4"/>
+      <c r="D1244" s="4"/>
+    </row>
+    <row r="1245" spans="1:4">
+      <c r="A1245" s="4" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B1245" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1245" s="4"/>
+      <c r="D1245" s="4"/>
+    </row>
+    <row r="1246" spans="1:4">
+      <c r="A1246" s="4" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B1246" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1246" s="4"/>
+      <c r="D1246" s="4"/>
+    </row>
+    <row r="1247" spans="1:4">
+      <c r="A1247" s="4" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B1247" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1247" s="4"/>
+      <c r="D1247" s="4"/>
+    </row>
+    <row r="1248" spans="1:4">
+      <c r="A1248" s="4" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B1248" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1248" s="4"/>
+      <c r="D1248" s="4"/>
+    </row>
+    <row r="1249" spans="1:4">
+      <c r="A1249" s="4" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B1249" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1249" s="4"/>
+      <c r="D1249" s="4"/>
+    </row>
+    <row r="1250" spans="1:4">
+      <c r="A1250" s="4" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B1250" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1250" s="4"/>
+      <c r="D1250" s="4"/>
+    </row>
+    <row r="1251" spans="1:4">
+      <c r="A1251" s="4" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B1251" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1251" s="4"/>
+      <c r="D1251" s="4"/>
+    </row>
+    <row r="1252" spans="1:4">
+      <c r="A1252" s="4" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B1252" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1252" s="4"/>
+      <c r="D1252" s="4"/>
+    </row>
+    <row r="1253" spans="1:4">
+      <c r="A1253" s="4" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B1253" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1253" s="4"/>
+      <c r="D1253" s="4"/>
+    </row>
+    <row r="1254" spans="1:4">
+      <c r="A1254" s="4" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1254" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1254" s="4"/>
+      <c r="D1254" s="4"/>
+    </row>
+    <row r="1255" spans="1:4">
+      <c r="A1255" s="4" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B1255" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1255" s="4"/>
+      <c r="D1255" s="4"/>
+    </row>
+    <row r="1256" spans="1:4">
+      <c r="A1256" s="4" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B1256" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1256" s="4"/>
+      <c r="D1256" s="4"/>
+    </row>
+    <row r="1257" spans="1:4">
+      <c r="A1257" s="4" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B1257" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1257" s="4"/>
+      <c r="D1257" s="4"/>
+    </row>
+    <row r="1258" spans="1:4">
+      <c r="A1258" s="4" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1258" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1258" s="4"/>
+      <c r="D1258" s="4"/>
+    </row>
+    <row r="1259" spans="1:4">
+      <c r="A1259" s="4" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B1259" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1259" s="4"/>
+      <c r="D1259" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>